<commit_message>
anik separated Asser regisyter
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/sample/depreciation.xlsx
+++ b/afar_project/csv_path/sample/depreciation.xlsx
@@ -583,7 +583,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0001</t>
+          <t>FRC-SLM-7-4-17-0001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0002</t>
+          <t>FRC-SLM-7-4-17-0002</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0003</t>
+          <t>FRC-SLM-7-4-17-0003</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0004</t>
+          <t>FRC-SLM-7-4-17-0004</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -995,7 +995,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0005</t>
+          <t>FRC-SLM-7-4-17-0005</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0006</t>
+          <t>FRC-SLM-7-4-17-0006</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0007</t>
+          <t>FRC-SLM-7-4-17-0007</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0008</t>
+          <t>FRC-SLM-7-4-17-0008</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0009</t>
+          <t>FRC-SLM-7-4-17-0009</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-17-0010</t>
+          <t>FRC-SLM-7-4-17-0010</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-17-0011</t>
+          <t>FRC-SLM-7-4-17-0011</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0012</t>
+          <t>FRC-SLM-7-4-17-0012</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0013</t>
+          <t>FRC-SLM-7-4-17-0013</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1909,7 +1909,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0014</t>
+          <t>FRC-SLM-7-4-17-0014</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0015</t>
+          <t>FRC-SLM-7-4-17-0015</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0016</t>
+          <t>FRC-SLM-7-4-17-0016</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0017</t>
+          <t>FRC-SLM-7-4-18-0017</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2281,10 +2281,10 @@
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>30145.79</v>
+        <v>30145.79439252336</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>-0.004392523358546896</v>
       </c>
       <c r="S18" t="n">
         <v>0.1</v>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0018</t>
+          <t>FRC-SLM-7-4-17-0018</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0019</t>
+          <t>FRC-SLM-7-4-17-0019</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0020</t>
+          <t>FRC-SLM-7-4-17-0020</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0021</t>
+          <t>FRC-SLM-7-4-17-0021</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0022</t>
+          <t>FRC-SLM-7-4-17-0022</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0023</t>
+          <t>FRC-SLM-7-4-17-0023</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0024</t>
+          <t>FRC-SLM-7-4-17-0024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0025</t>
+          <t>FRC-SLM-7-4-17-0025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0026</t>
+          <t>FRC-SLM-7-4-17-0026</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0027</t>
+          <t>FRC-SLM-7-4-17-0027</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -3351,7 +3351,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0028</t>
+          <t>FRC-SLM-7-4-17-0028</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0029</t>
+          <t>FRC-SLM-7-4-17-0029</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0030</t>
+          <t>FRC-SLM-7-4-17-0030</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0031</t>
+          <t>FRC-SLM-7-4-17-0031</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3763,7 +3763,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0032</t>
+          <t>FRC-SLM-7-4-18-0032</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0033</t>
+          <t>FRC-SLM-7-4-18-0033</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0034</t>
+          <t>FRC-SLM-7-4-18-0034</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0035</t>
+          <t>FRC-SLM-7-4-18-0035</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -4167,7 +4167,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0036</t>
+          <t>FRC-SLM-7-4-18-0036</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0037</t>
+          <t>FRC-SLM-7-4-17-0037</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -4375,7 +4375,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0038</t>
+          <t>FRC-SLM-7-4-18-0038</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0039</t>
+          <t>FRC-SLM-7-4-18-0039</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -4579,7 +4579,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0040</t>
+          <t>FRC-SLM-7-4-18-0040</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -4681,7 +4681,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0041</t>
+          <t>FRC-SLM-7-4-18-0041</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -4783,7 +4783,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0042</t>
+          <t>FRC-SLM-7-4-17-0042</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -4889,7 +4889,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0043</t>
+          <t>FRC-SLM-7-4-18-0043</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0044</t>
+          <t>FRC-SLM-7-4-18-0044</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-18-0045</t>
+          <t>FRC-SLM-7-4-18-0045</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-18-0046</t>
+          <t>FRC-SLM-7-4-18-0046</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0047</t>
+          <t>FRC-SLM-7-4-17-0047</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0048</t>
+          <t>FRC-SLM-7-4-17-0048</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -5507,7 +5507,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0049</t>
+          <t>FRC-SLM-7-4-18-0049</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0050</t>
+          <t>FRC-SLM-7-4-17-0050</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -5719,7 +5719,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0051</t>
+          <t>FRC-SLM-7-4-18-0051</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -5825,7 +5825,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0052</t>
+          <t>FRC-SLM-7-4-17-0052</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -5931,7 +5931,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0053</t>
+          <t>FRC-SLM-7-4-17-0053</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -6037,7 +6037,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0054</t>
+          <t>FRC-SLM-7-4-18-0054</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -6099,10 +6099,10 @@
         </is>
       </c>
       <c r="Q55" t="n">
-        <v>13789.8</v>
+        <v>13789.79591836735</v>
       </c>
       <c r="R55" t="n">
-        <v>0</v>
+        <v>0.004081632649103994</v>
       </c>
       <c r="S55" t="n">
         <v>0.1</v>
@@ -6143,7 +6143,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0055</t>
+          <t>FRC-SLM-7-4-18-0055</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -6249,7 +6249,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0056</t>
+          <t>FRC-SLM-7-4-18-0056</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -6355,7 +6355,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0057</t>
+          <t>FRC-SLM-7-4-18-0057</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0058</t>
+          <t>FRC-SLM-7-4-18-0058</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -6567,7 +6567,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0059</t>
+          <t>FRC-SLM-7-4-18-0059</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -6673,7 +6673,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0060</t>
+          <t>FRC-SLM-7-4-18-0060</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -6775,7 +6775,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0061</t>
+          <t>FRC-SLM-7-4-18-0061</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -6877,7 +6877,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0062</t>
+          <t>FRC-SLM-7-4-18-0062</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -6979,7 +6979,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0063</t>
+          <t>FRC-SLM-7-4-18-0063</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -7081,7 +7081,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0064</t>
+          <t>FRC-SLM-7-4-18-0064</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -7187,7 +7187,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0065</t>
+          <t>FRC-SLM-7-4-18-0065</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -7289,7 +7289,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0066</t>
+          <t>FRC-SLM-7-4-18-0066</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -7391,7 +7391,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0067</t>
+          <t>FRC-SLM-7-4-18-0067</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -7493,7 +7493,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0068</t>
+          <t>FRC-SLM-7-4-18-0068</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -7595,7 +7595,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0069</t>
+          <t>FRC-SLM-7-4-18-0069</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -7701,7 +7701,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0070</t>
+          <t>FRC-SLM-7-4-18-0070</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -7803,7 +7803,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0071</t>
+          <t>FRC-SLM-7-4-18-0071</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -7905,7 +7905,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0072</t>
+          <t>FRC-SLM-7-4-18-0072</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -8007,7 +8007,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0073</t>
+          <t>FRC-SLM-7-4-18-0073</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -8109,7 +8109,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0074</t>
+          <t>FRC-SLM-7-4-18-0074</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0075</t>
+          <t>FRC-SLM-7-4-18-0075</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -8313,7 +8313,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-18-0076</t>
+          <t>FRC-SLM-7-4-18-0076</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -8413,7 +8413,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0077</t>
+          <t>FRC-SLM-7-4-19-0077</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -8515,7 +8515,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0078</t>
+          <t>FRC-SLM-7-4-18-0078</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -8617,7 +8617,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0079</t>
+          <t>FRC-SLM-7-4-18-0079</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -8719,7 +8719,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0080</t>
+          <t>FRC-SLM-7-4-18-0080</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0081</t>
+          <t>FRC-SLM-7-4-18-0081</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -8923,7 +8923,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0082</t>
+          <t>FRC-SLM-7-4-18-0082</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -9025,7 +9025,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0083</t>
+          <t>FRC-SLM-7-4-18-0083</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -9127,7 +9127,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0084</t>
+          <t>FRC-SLM-7-4-18-0084</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -9229,7 +9229,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0085</t>
+          <t>FRC-SLM-7-4-18-0085</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -9331,7 +9331,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0086</t>
+          <t>FRC-SLM-7-4-18-0086</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -9433,7 +9433,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0087</t>
+          <t>FRC-SLM-7-4-18-0087</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -9535,7 +9535,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0088</t>
+          <t>FRC-SLM-7-4-18-0088</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -9637,7 +9637,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0089</t>
+          <t>FRC-SLM-7-4-18-0089</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -9739,7 +9739,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0090</t>
+          <t>FRC-SLM-7-4-18-0090</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -9841,7 +9841,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0091</t>
+          <t>FRC-SLM-7-4-18-0091</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -9947,7 +9947,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0092</t>
+          <t>FRC-SLM-7-4-18-0092</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -10053,7 +10053,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0093</t>
+          <t>FRC-SLM-7-4-18-0093</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -10159,7 +10159,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0094</t>
+          <t>FRC-SLM-7-4-19-0094</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -10265,7 +10265,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0095</t>
+          <t>FRC-SLM-7-4-18-0095</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -10365,7 +10365,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0096</t>
+          <t>FRC-SLM-7-4-19-0096</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -10467,7 +10467,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-19-0097</t>
+          <t>FRC-SLM-7-4-19-0097</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -10567,7 +10567,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-19-0098</t>
+          <t>FRC-SLM-7-4-19-0098</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -10669,7 +10669,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-19-0099</t>
+          <t>FRC-SLM-7-4-19-0099</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -10771,7 +10771,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0100</t>
+          <t>FRC-SLM-7-4-19-0100</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -10873,7 +10873,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0101</t>
+          <t>FRC-SLM-7-4-19-0101</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -10975,7 +10975,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0102</t>
+          <t>FRC-SLM-7-4-19-0102</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -11077,7 +11077,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0103</t>
+          <t>FRC-SLM-7-4-19-0103</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -11183,7 +11183,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0104</t>
+          <t>FRC-SLM-7-4-19-0104</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -11283,7 +11283,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0105</t>
+          <t>FRC-SLM-7-4-19-0105</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -11385,7 +11385,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0106</t>
+          <t>FRC-SLM-7-4-18-0106</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -11491,7 +11491,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0107</t>
+          <t>FRC-SLM-7-4-19-0107</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -11593,7 +11593,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0108</t>
+          <t>FRC-SLM-7-4-19-0108</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -11695,7 +11695,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0109</t>
+          <t>FRC-SLM-7-4-19-0109</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -11797,7 +11797,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0110</t>
+          <t>FRC-SLM-7-4-19-0110</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -11903,7 +11903,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0111</t>
+          <t>FRC-SLM-7-4-19-0111</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -12009,7 +12009,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0112</t>
+          <t>FRC-SLM-7-4-20-0112</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -12115,7 +12115,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0113</t>
+          <t>FRC-SLM-7-4-19-0113</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -12221,7 +12221,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0114</t>
+          <t>FRC-SLM-7-4-19-0114</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0115</t>
+          <t>FRC-SLM-7-4-19-0115</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -12425,7 +12425,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0116</t>
+          <t>FRC-SLM-7-4-19-0116</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -12527,7 +12527,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0117</t>
+          <t>FRC-SLM-7-4-19-0117</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -12633,7 +12633,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0118</t>
+          <t>FRC-SLM-7-4-19-0118</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -12735,7 +12735,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0119</t>
+          <t>FRC-SLM-7-4-19-0119</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -12837,7 +12837,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0120</t>
+          <t>FRC-SLM-7-4-19-0120</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -12939,7 +12939,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0121</t>
+          <t>FRC-SLM-7-4-19-0121</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -13041,7 +13041,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0122</t>
+          <t>FRC-SLM-7-4-19-0122</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -13143,7 +13143,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0123</t>
+          <t>FRC-SLM-7-4-19-0123</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -13245,7 +13245,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0124</t>
+          <t>FRC-SLM-7-4-19-0124</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -13347,7 +13347,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0125</t>
+          <t>FRC-SLM-7-4-19-0125</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -13449,7 +13449,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0126</t>
+          <t>FRC-SLM-7-4-20-0126</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -13551,7 +13551,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0127</t>
+          <t>FRC-SLM-7-4-20-0127</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -13653,7 +13653,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0128</t>
+          <t>FRC-SLM-7-4-20-0128</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -13755,7 +13755,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0129</t>
+          <t>FRC-SLM-7-4-20-0129</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -13857,7 +13857,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0130</t>
+          <t>FRC-SLM-7-4-20-0130</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -13959,7 +13959,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0131</t>
+          <t>FRC-SLM-7-4-20-0131</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -14061,7 +14061,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0132</t>
+          <t>FRC-SLM-7-4-20-0132</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -14163,7 +14163,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-20-0133</t>
+          <t>FRC-SLM-7-4-20-0133</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -14265,7 +14265,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0134</t>
+          <t>FRC-SLM-7-4-21-0134</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -14367,7 +14367,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0135</t>
+          <t>FRC-SLM-7-4-21-0135</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -14469,7 +14469,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0136</t>
+          <t>FRC-SLM-7-4-21-0136</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -14571,7 +14571,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0137</t>
+          <t>FRC-SLM-7-4-21-0137</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -14673,7 +14673,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0138</t>
+          <t>FRC-SLM-7-4-21-0138</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -14775,7 +14775,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0139</t>
+          <t>FRC-SLM-7-4-21-0139</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -14877,7 +14877,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0140</t>
+          <t>FRC-SLM-7-4-21-0140</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -14979,7 +14979,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0141</t>
+          <t>FRC-SLM-7-4-21-0141</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -15081,7 +15081,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0142</t>
+          <t>FRC-SLM-7-4-21-0142</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -15183,7 +15183,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0143</t>
+          <t>FRC-SLM-7-4-21-0143</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -15285,7 +15285,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0144</t>
+          <t>FRC-SLM-7-4-21-0144</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -15385,7 +15385,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-22-0145</t>
+          <t>FRC-SLM-7-4-22-0145</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -15487,7 +15487,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0146</t>
+          <t>FRC-SLM-7-4-22-0146</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -15589,7 +15589,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0147</t>
+          <t>FRC-SLM-7-4-22-0147</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -15691,7 +15691,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-22-0148</t>
+          <t>FRC-SLM-7-4-22-0148</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -15791,7 +15791,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0149</t>
+          <t>FRC-SLM-7-4-22-0149</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -15893,7 +15893,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-22-0150</t>
+          <t>FRC-SLM-7-4-22-0150</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -15995,7 +15995,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0152</t>
+          <t>FRC-SLM-7-n-22-0152</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -16099,7 +16099,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0153</t>
+          <t>FRC-SLM-7-n-22-0153</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -16203,7 +16203,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0154</t>
+          <t>FRC-SLM-7-n-22-0154</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -16307,7 +16307,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0155</t>
+          <t>FRC-SLM-7-n-22-0155</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -16411,7 +16411,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0156</t>
+          <t>FRC-SLM-7-n-22-0156</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -16515,7 +16515,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0157</t>
+          <t>FRC-SLM-7-n-22-0157</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -16619,7 +16619,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0158</t>
+          <t>FRC-SLM-7-n-22-0158</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -16723,7 +16723,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0159</t>
+          <t>FRC-SLM-7-n-22-0159</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -16827,7 +16827,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0160</t>
+          <t>FRC-SLM-7-n-22-0160</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -16931,7 +16931,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0161</t>
+          <t>FRC-SLM-7-n-22-0161</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -17035,7 +17035,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0162</t>
+          <t>FRC-SLM-7-n-22-0162</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -17139,7 +17139,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0163</t>
+          <t>FRC-SLM-7-n-22-0163</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -17243,7 +17243,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0164</t>
+          <t>FRC-SLM-7-n-22-0164</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -17347,7 +17347,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0165</t>
+          <t>FRC-SLM-7-n-22-0165</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -17451,7 +17451,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0166</t>
+          <t>FRC-SLM-7-n-22-0166</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -17555,7 +17555,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0167</t>
+          <t>FRC-SLM-7-n-22-0167</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -17659,7 +17659,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0168</t>
+          <t>FRC-SLM-7-n-22-0168</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -17763,7 +17763,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0169</t>
+          <t>FRC-SLM-7-n-22-0169</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -17868,7 +17868,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0170</t>
+          <t>FRC-SLM-7-n-22-0170</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -17972,7 +17972,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0171</t>
+          <t>FRC-SLM-7-n-22-0171</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -18076,7 +18076,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0172</t>
+          <t>FRC-SLM-7-n-22-0172</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -18180,7 +18180,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0173</t>
+          <t>FRC-SLM-7-n-22-0173</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -18284,7 +18284,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0174</t>
+          <t>FRC-SLM-7-n-22-0174</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -18388,7 +18388,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0175</t>
+          <t>FRC-SLM-7-n-22-0175</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -18492,7 +18492,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0176</t>
+          <t>FRC-SLM-7-n-22-0176</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -18596,7 +18596,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0177</t>
+          <t>FRC-SLM-7-n-22-0177</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -18700,7 +18700,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0178</t>
+          <t>FRC-SLM-7-n-22-0178</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -18804,7 +18804,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0179</t>
+          <t>FRC-SLM-7-n-22-0179</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -18908,7 +18908,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0180</t>
+          <t>FRC-SLM-7-n-22-0180</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -19012,7 +19012,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0181</t>
+          <t>FRC-SLM-7-n-22-0181</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -19116,7 +19116,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0182</t>
+          <t>FRC-SLM-7-n-22-0182</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -19220,7 +19220,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0183</t>
+          <t>FRC-SLM-7-n-22-0183</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -19324,7 +19324,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0184</t>
+          <t>FRC-SLM-7-n-22-0184</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -19429,7 +19429,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0185</t>
+          <t>FRC-SLM-7-n-22-0185</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -19533,7 +19533,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0186</t>
+          <t>FRC-SLM-7-n-22-0186</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -19637,7 +19637,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0187</t>
+          <t>FRC-SLM-7-n-22-0187</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -19741,7 +19741,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0188</t>
+          <t>FRC-SLM-7-n-22-0188</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -19845,7 +19845,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0189</t>
+          <t>FRC-SLM-7-n-22-0189</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -19949,7 +19949,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0190</t>
+          <t>FRC-SLM-7-n-22-0190</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -20053,7 +20053,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0191</t>
+          <t>FRC-SLM-7-n-22-0191</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -20157,7 +20157,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0192</t>
+          <t>FRC-SLM-7-n-22-0192</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -20261,7 +20261,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0193</t>
+          <t>FRC-SLM-7-n-22-0193</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -20365,7 +20365,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0194</t>
+          <t>FRC-SLM-7-n-22-0194</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -20469,7 +20469,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0195</t>
+          <t>FRC-SLM-7-n-22-0195</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -20573,7 +20573,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0196</t>
+          <t>FRC-SLM-7-n-22-0196</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -20677,7 +20677,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-22-0197</t>
+          <t>FRC-SLM-7-n-22-0197</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -20781,7 +20781,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0198</t>
+          <t>FRC-SLM-7-n-22-0198</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -20885,7 +20885,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0199</t>
+          <t>FRC-SLM-7-n-22-0199</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -20989,7 +20989,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0200</t>
+          <t>FRC-SLM-7-n-22-0200</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -21093,7 +21093,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0201</t>
+          <t>FRC-SLM-7-n-22-0201</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -21197,7 +21197,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0202</t>
+          <t>FRC-SLM-7-n-22-0202</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -21301,7 +21301,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0203</t>
+          <t>FRC-SLM-7-n-22-0203</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -21405,7 +21405,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0204</t>
+          <t>FRC-SLM-7-n-22-0204</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -21509,7 +21509,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0205</t>
+          <t>FRC-SLM-7-n-22-0205</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -21613,7 +21613,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0206</t>
+          <t>FRC-SLM-7-n-22-0206</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -21717,7 +21717,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0207</t>
+          <t>FRC-SLM-7-n-22-0207</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -21821,7 +21821,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0208</t>
+          <t>FRC-SLM-7-n-22-0208</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -21925,7 +21925,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0209</t>
+          <t>FRC-SLM-7-n-22-0209</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -22029,7 +22029,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0210</t>
+          <t>FRC-SLM-7-n-22-0210</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -22133,7 +22133,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0211</t>
+          <t>FRC-SLM-7-n-22-0211</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -22237,7 +22237,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0212</t>
+          <t>FRC-SLM-7-n-22-0212</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -22341,7 +22341,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0213</t>
+          <t>FRC-SLM-7-n-22-0213</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -22445,7 +22445,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0214</t>
+          <t>FRC-SLM-7-n-22-0214</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -22549,7 +22549,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0215</t>
+          <t>FRC-SLM-7-n-22-0215</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -22653,7 +22653,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0216</t>
+          <t>FRC-SLM-7-n-22-0216</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -22757,7 +22757,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0217</t>
+          <t>FRC-SLM-7-n-22-0217</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -22861,7 +22861,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0218</t>
+          <t>FRC-SLM-7-n-22-0218</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -22965,7 +22965,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0219</t>
+          <t>FRC-SLM-7-n-22-0219</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -23069,7 +23069,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0220</t>
+          <t>FRC-SLM-7-n-22-0220</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -23173,7 +23173,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0221</t>
+          <t>FRC-SLM-7-n-22-0221</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -23277,7 +23277,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0222</t>
+          <t>FRC-SLM-7-n-22-0222</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -23381,7 +23381,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0223</t>
+          <t>FRC-SLM-7-n-22-0223</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -23485,7 +23485,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0224</t>
+          <t>FRC-SLM-7-n-22-0224</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -23589,7 +23589,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0225</t>
+          <t>FRC-SLM-7-n-22-0225</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -23693,7 +23693,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0226</t>
+          <t>FRC-SLM-7-n-22-0226</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -23797,7 +23797,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0227</t>
+          <t>FRC-SLM-7-n-22-0227</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -23901,7 +23901,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0228</t>
+          <t>FRC-SLM-7-n-22-0228</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -24005,7 +24005,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0229</t>
+          <t>FRC-SLM-7-n-22-0229</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -24109,7 +24109,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0230</t>
+          <t>FRC-SLM-7-n-22-0230</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -24213,7 +24213,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0231</t>
+          <t>FRC-SLM-7-n-22-0231</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -24317,7 +24317,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0232</t>
+          <t>FRC-SLM-7-n-22-0232</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -24421,7 +24421,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0233</t>
+          <t>FRC-SLM-7-n-22-0233</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -24525,7 +24525,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0234</t>
+          <t>FRC-SLM-7-n-22-0234</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -24629,7 +24629,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0235</t>
+          <t>FRC-SLM-7-n-22-0235</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -24733,7 +24733,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-22-0236</t>
+          <t>FRC-SLM-7-n-22-0236</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -24837,7 +24837,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-22-0237</t>
+          <t>FRC-SLM-7-n-22-0237</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -24941,7 +24941,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-22-0238</t>
+          <t>FRC-SLM-7-n-22-0238</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -25045,7 +25045,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-22-0239</t>
+          <t>FRC-SLM-7-n-22-0239</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -25149,7 +25149,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-22-0240</t>
+          <t>FRC-SLM-7-n-22-0240</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -25253,7 +25253,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-22-0241</t>
+          <t>FRC-SLM-7-n-22-0241</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -25357,7 +25357,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0242</t>
+          <t>FRC-SLM-7-n-22-0242</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -25461,7 +25461,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0243</t>
+          <t>FRC-SLM-7-n-22-0243</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -25565,7 +25565,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0244</t>
+          <t>FRC-SLM-7-n-22-0244</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -25669,7 +25669,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0245</t>
+          <t>FRC-SLM-7-n-22-0245</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -25773,7 +25773,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0246</t>
+          <t>FRC-SLM-7-n-22-0246</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -25877,7 +25877,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0247</t>
+          <t>FRC-SLM-7-n-22-0247</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -25981,7 +25981,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0248</t>
+          <t>FRC-SLM-7-n-22-0248</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -26085,7 +26085,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0249</t>
+          <t>FRC-SLM-7-n-22-0249</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -26189,7 +26189,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0250</t>
+          <t>FRC-SLM-7-n-22-0250</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -26293,7 +26293,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0251</t>
+          <t>FRC-SLM-7-n-22-0251</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -26397,7 +26397,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0252</t>
+          <t>FRC-SLM-7-n-22-0252</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -26501,7 +26501,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0253</t>
+          <t>FRC-SLM-7-n-22-0253</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -26605,7 +26605,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0254</t>
+          <t>FRC-SLM-7-n-22-0254</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -26709,7 +26709,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0255</t>
+          <t>FRC-SLM-7-n-22-0255</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -26813,7 +26813,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0256</t>
+          <t>FRC-SLM-7-n-22-0256</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -26917,7 +26917,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0257</t>
+          <t>FRC-SLM-7-n-22-0257</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -27021,7 +27021,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0258</t>
+          <t>FRC-SLM-7-n-22-0258</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -27125,7 +27125,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0259</t>
+          <t>FRC-SLM-7-n-22-0259</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -27229,7 +27229,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0260</t>
+          <t>FRC-SLM-7-n-22-0260</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -27333,7 +27333,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0261</t>
+          <t>FRC-SLM-7-n-22-0261</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -27437,7 +27437,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0262</t>
+          <t>FRC-SLM-7-n-22-0262</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -27541,7 +27541,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0263</t>
+          <t>FRC-SLM-7-n-22-0263</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -27645,7 +27645,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0264</t>
+          <t>FRC-SLM-7-n-22-0264</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -27749,7 +27749,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0265</t>
+          <t>FRC-SLM-7-n-22-0265</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -27853,7 +27853,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0266</t>
+          <t>FRC-SLM-7-n-22-0266</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -27957,7 +27957,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0267</t>
+          <t>FRC-SLM-7-n-22-0267</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -28061,7 +28061,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0268</t>
+          <t>FRC-SLM-7-n-22-0268</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -28165,7 +28165,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0269</t>
+          <t>FRC-SLM-7-n-22-0269</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -28269,7 +28269,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0270</t>
+          <t>FRC-SLM-7-n-22-0270</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -28373,7 +28373,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0271</t>
+          <t>FRC-SLM-7-n-22-0271</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -28477,7 +28477,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0272</t>
+          <t>FRC-SLM-7-n-22-0272</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -28581,7 +28581,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0273</t>
+          <t>FRC-SLM-7-n-22-0273</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -28685,7 +28685,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-22-0274</t>
+          <t>FRC-SLM-7-n-22-0274</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -28789,7 +28789,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0275</t>
+          <t>FRC-SLM-7-n-22-0275</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -28893,7 +28893,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0276</t>
+          <t>FRC-SLM-7-n-22-0276</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -28997,7 +28997,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0277</t>
+          <t>FRC-SLM-7-n-22-0277</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -29101,7 +29101,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0278</t>
+          <t>FRC-SLM-7-n-22-0278</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -29205,7 +29205,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0279</t>
+          <t>FRC-SLM-7-n-22-0279</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -29309,7 +29309,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0280</t>
+          <t>FRC-SLM-7-n-22-0280</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -29413,7 +29413,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0281</t>
+          <t>FRC-SLM-7-n-22-0281</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -29517,7 +29517,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0282</t>
+          <t>FRC-SLM-7-n-22-0282</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -29621,7 +29621,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0283</t>
+          <t>FRC-SLM-7-n-22-0283</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -29725,7 +29725,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0284</t>
+          <t>FRC-SLM-7-n-22-0284</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -29829,7 +29829,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0285</t>
+          <t>FRC-SLM-7-n-22-0285</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -29933,7 +29933,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0286</t>
+          <t>FRC-SLM-7-n-22-0286</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -30037,7 +30037,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0287</t>
+          <t>FRC-SLM-7-n-22-0287</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -30141,7 +30141,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0288</t>
+          <t>FRC-SLM-7-n-22-0288</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -30245,7 +30245,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0289</t>
+          <t>FRC-SLM-7-n-22-0289</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -30349,7 +30349,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0290</t>
+          <t>FRC-SLM-7-n-22-0290</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -30453,7 +30453,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0291</t>
+          <t>FRC-SLM-7-n-22-0291</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -30557,7 +30557,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0292</t>
+          <t>FRC-SLM-7-n-22-0292</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -30661,7 +30661,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0293</t>
+          <t>FRC-SLM-7-n-22-0293</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -30765,7 +30765,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0294</t>
+          <t>FRC-SLM-7-n-22-0294</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -30869,7 +30869,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0295</t>
+          <t>FRC-SLM-7-n-22-0295</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -30973,7 +30973,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0296</t>
+          <t>FRC-SLM-7-n-22-0296</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -31077,7 +31077,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0297</t>
+          <t>FRC-SLM-7-n-22-0297</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -31181,7 +31181,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0298</t>
+          <t>FRC-SLM-7-n-22-0298</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -31285,7 +31285,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0299</t>
+          <t>FRC-SLM-7-n-22-0299</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -31389,7 +31389,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0300</t>
+          <t>FRC-SLM-7-n-22-0300</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -31493,7 +31493,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-22-0301</t>
+          <t>FRC-SLM-7-n-22-0301</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">

</xml_diff>